<commit_message>
add scripts to find test poses
</commit_message>
<xml_diff>
--- a/target_poses.xlsx
+++ b/target_poses.xlsx
@@ -350,8 +350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -373,7 +373,7 @@
         <v>0.02</v>
       </c>
       <c r="F1">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="G1">
         <v>0</v>
@@ -435,7 +435,7 @@
         <v>0.03</v>
       </c>
       <c r="F2">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -444,7 +444,7 @@
         <v>-0.05</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -692,7 +692,7 @@
         <v>0.05</v>
       </c>
       <c r="I6">
-        <v>-0.15</v>
+        <v>0.06</v>
       </c>
       <c r="J6">
         <v>-0.1</v>

</xml_diff>